<commit_message>
organized the order of stories
</commit_message>
<xml_diff>
--- a/DesignDocs/Economy.xlsx
+++ b/DesignDocs/Economy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Unity 2D\GreatGame\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6633474C-5264-48AA-9B87-C1D4F146840B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BB4733-D227-4709-9CA4-366C669DF2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D173FA28-FAEC-4CF8-9DAD-031960158530}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Places</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +95,50 @@
   </si>
   <si>
     <t>Best Case</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Astrakan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Krasnovodsk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turcomans passing by</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meeting a thirsty turcoman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turcoman selling supplies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turcoman bandit raid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extreme heat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Major Frankenburg verge of death</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oasis Mirage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Real Oasis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strong heat causing thirst</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -304,22 +348,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -374,16 +418,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10</c:v>
@@ -1159,13 +1203,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>252412</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>33337</xdr:rowOff>
@@ -1513,44 +1557,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE9C84E-51C7-4ACB-B5F4-C9F30504F147}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1566,17 +1611,17 @@
       <c r="F6" t="s">
         <v>3</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>10</v>
-      </c>
-      <c r="I6">
-        <v>60</v>
       </c>
       <c r="J6">
         <v>60</v>
       </c>
+      <c r="K6">
+        <v>60</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1592,19 +1637,22 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
         <v>5</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f>SUM(B18,E18)</f>
         <v>84</v>
       </c>
-      <c r="J7">
-        <f>I7-21</f>
+      <c r="K7">
+        <f>J7-21</f>
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1620,18 +1668,21 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
         <v>6</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f>F18</f>
+        <v>16</v>
+      </c>
+      <c r="K8">
         <v>22</v>
       </c>
-      <c r="J8">
-        <v>22</v>
-      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1642,24 +1693,27 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
         <v>11</v>
-      </c>
-      <c r="I9">
-        <f>I6-I7+I8</f>
-        <v>-2</v>
       </c>
       <c r="J9">
         <f>J6-J7+J8</f>
+        <v>-8</v>
+      </c>
+      <c r="K9">
+        <f>K6-K7+K8</f>
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1670,13 +1724,16 @@
         <v>4</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1687,13 +1744,16 @@
         <v>5</v>
       </c>
       <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
         <v>0</v>
       </c>
-      <c r="F11">
-        <v>4</v>
+      <c r="G11" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1704,13 +1764,16 @@
         <v>6</v>
       </c>
       <c r="E12">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7</v>
       </c>
@@ -1721,13 +1784,16 @@
         <v>7</v>
       </c>
       <c r="E13">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1738,13 +1804,16 @@
         <v>8</v>
       </c>
       <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14">
         <v>0</v>
       </c>
-      <c r="F14">
-        <v>8</v>
+      <c r="G14" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1760,8 +1829,11 @@
       <c r="F15">
         <v>10</v>
       </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1777,8 +1849,11 @@
       <c r="F16">
         <v>0</v>
       </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>11</v>
       </c>
@@ -1794,8 +1869,11 @@
       <c r="F17">
         <v>0</v>
       </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1812,7 +1890,7 @@
       </c>
       <c r="F18">
         <f>SUM(F7:F17)</f>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
notes added, design docs updated
</commit_message>
<xml_diff>
--- a/DesignDocs/Economy.xlsx
+++ b/DesignDocs/Economy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Unity 2D\GreatGame\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BB4733-D227-4709-9CA4-366C669DF2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2881B04E-95A3-4DBB-AC0E-33D81334E80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D173FA28-FAEC-4CF8-9DAD-031960158530}"/>
+    <workbookView xWindow="28935" yWindow="3285" windowWidth="21600" windowHeight="11385" xr2:uid="{D173FA28-FAEC-4CF8-9DAD-031960158530}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -284,31 +284,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -351,28 +351,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -421,7 +421,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -430,7 +430,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1565,6 +1565,8 @@
   <cols>
     <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1615,10 +1617,11 @@
         <v>10</v>
       </c>
       <c r="J6">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="K6">
-        <v>60</v>
+        <f>J6</f>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1645,11 +1648,11 @@
       </c>
       <c r="J7">
         <f>SUM(B18,E18)</f>
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="K7">
         <f>J7-21</f>
-        <v>63</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1676,7 +1679,7 @@
       </c>
       <c r="J8">
         <f>F18</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K8">
         <v>22</v>
@@ -1687,7 +1690,7 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -1706,11 +1709,11 @@
       </c>
       <c r="J9">
         <f>J6-J7+J8</f>
-        <v>-8</v>
+        <v>-3</v>
       </c>
       <c r="K9">
         <f>K6-K7+K8</f>
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1718,13 +1721,13 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>4</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1738,13 +1741,13 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>5</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1758,7 +1761,7 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -1767,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
@@ -1778,13 +1781,13 @@
         <v>7</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>7</v>
       </c>
       <c r="E13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1798,13 +1801,13 @@
         <v>8</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>8</v>
       </c>
       <c r="E14">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1818,7 +1821,7 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <v>9</v>
@@ -1827,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
@@ -1838,13 +1841,13 @@
         <v>10</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <v>10</v>
       </c>
       <c r="E16">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1858,13 +1861,13 @@
         <v>11</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <v>11</v>
       </c>
       <c r="E17">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1879,18 +1882,18 @@
       </c>
       <c r="B18">
         <f>SUM(B7:B17)</f>
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
       </c>
       <c r="E18">
         <f>SUM(E7:E17)</f>
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="F18">
         <f>SUM(F7:F17)</f>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
background concept table added
</commit_message>
<xml_diff>
--- a/DesignDocs/Economy.xlsx
+++ b/DesignDocs/Economy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Unity 2D\GreatGame\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2881B04E-95A3-4DBB-AC0E-33D81334E80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB0C9E8-9EA1-480D-841E-3CE7B1FC5C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28935" yWindow="3285" windowWidth="21600" windowHeight="11385" xr2:uid="{D173FA28-FAEC-4CF8-9DAD-031960158530}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D173FA28-FAEC-4CF8-9DAD-031960158530}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1563,7 +1563,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
@@ -1589,14 +1589,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
@@ -1613,15 +1605,11 @@
       <c r="F6" t="s">
         <v>3</v>
       </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>40</v>
-      </c>
-      <c r="K6">
-        <f>J6</f>
-        <v>40</v>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1644,15 +1632,14 @@
         <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J7">
-        <f>SUM(B18,E18)</f>
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="K7">
-        <f>J7-21</f>
-        <v>36</v>
+        <f>J7</f>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1675,14 +1662,15 @@
         <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J8">
-        <f>F18</f>
-        <v>14</v>
+        <f>SUM(B18,E18)</f>
+        <v>57</v>
       </c>
       <c r="K8">
-        <v>22</v>
+        <f>J8-21</f>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1705,15 +1693,14 @@
         <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J9">
-        <f>J6-J7+J8</f>
-        <v>-3</v>
+        <f>F18</f>
+        <v>14</v>
       </c>
       <c r="K9">
-        <f>K6-K7+K8</f>
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1734,6 +1721,17 @@
       </c>
       <c r="G10" t="s">
         <v>18</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10">
+        <f>J7-J8+J9</f>
+        <v>-3</v>
+      </c>
+      <c r="K10">
+        <f>K7-K8+K9</f>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
trust point design ideas added
</commit_message>
<xml_diff>
--- a/DesignDocs/Economy.xlsx
+++ b/DesignDocs/Economy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Unity 2D\GreatGame\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C5D27D-A1A7-4DEF-A46B-6ABF4967339B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700F2B80-522A-4BC3-9620-60CA90289110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D173FA28-FAEC-4CF8-9DAD-031960158530}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{D173FA28-FAEC-4CF8-9DAD-031960158530}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Places</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,6 +139,10 @@
   </si>
   <si>
     <t>Provide water just enough to survive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*Yellow is where trust point may be gained or lost</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -163,12 +167,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -185,8 +195,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1563,7 +1576,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
@@ -1605,6 +1618,9 @@
       <c r="F6" t="s">
         <v>3</v>
       </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
       <c r="J6" t="s">
         <v>11</v>
       </c>
@@ -1628,7 +1644,7 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I7" t="s">
@@ -1658,7 +1674,7 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I8" t="s">
@@ -1790,7 +1806,7 @@
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>